<commit_message>
Added rest of MLP studies and created SVM script
</commit_message>
<xml_diff>
--- a/Coursework - Commercial/LR_tst_results.xlsx
+++ b/Coursework - Commercial/LR_tst_results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="32">
   <si>
     <t>configuration</t>
   </si>
@@ -134,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -148,11 +148,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -160,6 +166,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,7 +214,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true"/>
     <col min="8" max="8" width="12.7109375" customWidth="true"/>
     <col min="9" max="9" width="5.140625" customWidth="true"/>
     <col min="10" max="10" width="5.140625" customWidth="true"/>
@@ -211,798 +223,801 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.54746136865342165</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.65495011511895629</v>
+      </c>
+      <c r="D2">
+        <v>0.58918128654970758</v>
       </c>
       <c r="E2">
-        <v>0.52523379554982264</v>
+        <v>0.61555106751298327</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.45253863134657835</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.34504988488104377</v>
       </c>
       <c r="H2">
-        <v>0.52523379554982264</v>
+        <v>0.60391809093840698</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>3224</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>2248</v>
       </c>
       <c r="K2">
-        <v>6515</v>
+        <v>4267</v>
       </c>
       <c r="L2">
-        <v>5889</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.49516046867040242</v>
+        <v>0.35472915605365934</v>
       </c>
       <c r="C3">
-        <v>0.89148119723714503</v>
+        <v>0.93415195702225629</v>
       </c>
       <c r="D3">
-        <v>0.80485785260833564</v>
+        <v>0.82962668784749805</v>
       </c>
       <c r="E3">
-        <v>0.66142808336180392</v>
+        <v>0.61561804572122192</v>
       </c>
       <c r="F3">
-        <v>0.50483953132959758</v>
+        <v>0.6452708439463406</v>
       </c>
       <c r="G3">
-        <v>0.10851880276285494</v>
+        <v>0.065848042977743673</v>
       </c>
       <c r="H3">
-        <v>0.70332150919058367</v>
+        <v>0.65906159303450496</v>
       </c>
       <c r="I3">
-        <v>2916</v>
+        <v>2089</v>
       </c>
       <c r="J3">
-        <v>707</v>
+        <v>429</v>
       </c>
       <c r="K3">
-        <v>5808</v>
+        <v>6086</v>
       </c>
       <c r="L3">
-        <v>2973</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.67889285107828157</v>
+        <v>0.67566649685854985</v>
       </c>
       <c r="C4">
-        <v>0.82256331542594019</v>
+        <v>0.82409823484267075</v>
       </c>
       <c r="D4">
-        <v>0.77570818781528905</v>
+        <v>0.77639024390243905</v>
       </c>
       <c r="E4">
-        <v>0.7391724137931035</v>
+        <v>0.73760131886248115</v>
       </c>
       <c r="F4">
-        <v>0.32110714892171843</v>
+        <v>0.32433350314145015</v>
       </c>
       <c r="G4">
-        <v>0.17743668457405987</v>
+        <v>0.17590176515732925</v>
       </c>
       <c r="H4">
-        <v>0.75435343437600777</v>
+        <v>0.75362786198000642</v>
       </c>
       <c r="I4">
-        <v>3998</v>
+        <v>3979</v>
       </c>
       <c r="J4">
-        <v>1156</v>
+        <v>1146</v>
       </c>
       <c r="K4">
-        <v>5359</v>
+        <v>5369</v>
       </c>
       <c r="L4">
-        <v>1891</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.75021226014603493</v>
+        <v>0.74783494651044324</v>
       </c>
       <c r="C5">
-        <v>0.77651573292402154</v>
+        <v>0.77881811204911744</v>
       </c>
       <c r="D5">
-        <v>0.75212802179094318</v>
+        <v>0.75346449957228401</v>
       </c>
       <c r="E5">
-        <v>0.77473200612557425</v>
+        <v>0.77359353559993904</v>
       </c>
       <c r="F5">
-        <v>0.24978773985396502</v>
+        <v>0.25216505348955681</v>
       </c>
       <c r="G5">
-        <v>0.22348426707597852</v>
+        <v>0.22118188795088259</v>
       </c>
       <c r="H5">
-        <v>0.76402773298935822</v>
+        <v>0.76410835214446948</v>
       </c>
       <c r="I5">
-        <v>4418</v>
+        <v>4404</v>
       </c>
       <c r="J5">
-        <v>1456</v>
+        <v>1441</v>
       </c>
       <c r="K5">
-        <v>5059</v>
+        <v>5074</v>
       </c>
       <c r="L5">
-        <v>1471</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>0.739174732552216</v>
+      </c>
+      <c r="C6">
+        <v>0.81995395241749813</v>
+      </c>
+      <c r="D6">
+        <v>0.78773072747014117</v>
+      </c>
+      <c r="E6">
+        <v>0.77667926722884562</v>
+      </c>
+      <c r="F6">
+        <v>0.260825267447784</v>
+      </c>
+      <c r="G6">
+        <v>0.18004604758250192</v>
+      </c>
+      <c r="H6">
+        <v>0.78160270880361171</v>
+      </c>
+      <c r="I6">
+        <v>4353</v>
+      </c>
+      <c r="J6">
+        <v>1173</v>
+      </c>
+      <c r="K6">
+        <v>5342</v>
+      </c>
+      <c r="L6">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.73272202411275256</v>
+      </c>
+      <c r="C7">
+        <v>0.8409823484267076</v>
+      </c>
+      <c r="D7">
+        <v>0.80639132872360308</v>
+      </c>
+      <c r="E7">
+        <v>0.77683255352332337</v>
+      </c>
+      <c r="F7">
+        <v>0.26727797588724739</v>
+      </c>
+      <c r="G7">
+        <v>0.1590176515732924</v>
+      </c>
+      <c r="H7">
+        <v>0.7895840051596259</v>
+      </c>
+      <c r="I7">
+        <v>4315</v>
+      </c>
+      <c r="J7">
+        <v>1036</v>
+      </c>
+      <c r="K7">
+        <v>5479</v>
+      </c>
+      <c r="L7">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.73374087281372047</v>
+      </c>
+      <c r="C8">
+        <v>0.85326170376055255</v>
+      </c>
+      <c r="D8">
+        <v>0.81883646010991096</v>
+      </c>
+      <c r="E8">
+        <v>0.77999158131050939</v>
+      </c>
+      <c r="F8">
+        <v>0.26625912718627953</v>
+      </c>
+      <c r="G8">
+        <v>0.14673829623944742</v>
+      </c>
+      <c r="H8">
+        <v>0.79651725249919381</v>
+      </c>
+      <c r="I8">
+        <v>4321</v>
+      </c>
+      <c r="J8">
+        <v>956</v>
+      </c>
+      <c r="K8">
+        <v>5559</v>
+      </c>
+      <c r="L8">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.73696722703345219</v>
+      </c>
+      <c r="C9">
+        <v>0.86523407521105145</v>
+      </c>
+      <c r="D9">
+        <v>0.83173629743196631</v>
+      </c>
+      <c r="E9">
+        <v>0.78444197049819098</v>
+      </c>
+      <c r="F9">
+        <v>0.26303277296654781</v>
+      </c>
+      <c r="G9">
+        <v>0.13476592478894858</v>
+      </c>
+      <c r="H9">
+        <v>0.80433731054498547</v>
+      </c>
+      <c r="I9">
+        <v>4340</v>
+      </c>
+      <c r="J9">
+        <v>878</v>
+      </c>
+      <c r="K9">
+        <v>5637</v>
+      </c>
+      <c r="L9">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>0.74087281372049585</v>
       </c>
-      <c r="C6">
-        <v>0.81688411358403679</v>
-      </c>
-      <c r="D6">
-        <v>0.78527717782577389</v>
-      </c>
-      <c r="E6">
-        <v>0.77716121495327106</v>
-      </c>
-      <c r="F6">
+      <c r="C10">
+        <v>0.86999232540291638</v>
+      </c>
+      <c r="D10">
+        <v>0.83742802303262953</v>
+      </c>
+      <c r="E10">
+        <v>0.78787878787878785</v>
+      </c>
+      <c r="F10">
         <v>0.25912718627950415</v>
       </c>
-      <c r="G6">
-        <v>0.18311588641596316</v>
-      </c>
-      <c r="H6">
-        <v>0.78079651725249921</v>
-      </c>
-      <c r="I6">
+      <c r="G10">
+        <v>0.13000767459708365</v>
+      </c>
+      <c r="H10">
+        <v>0.80869074492099324</v>
+      </c>
+      <c r="I10">
         <v>4363</v>
       </c>
-      <c r="J6">
-        <v>1193</v>
-      </c>
-      <c r="K6">
-        <v>5322</v>
-      </c>
-      <c r="L6">
+      <c r="J10">
+        <v>847</v>
+      </c>
+      <c r="K10">
+        <v>5668</v>
+      </c>
+      <c r="L10">
         <v>1526</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.7367974189166242</v>
-      </c>
-      <c r="C7">
-        <v>0.83315425940138144</v>
-      </c>
-      <c r="D7">
-        <v>0.79966826391448576</v>
-      </c>
-      <c r="E7">
-        <v>0.77787331613642874</v>
-      </c>
-      <c r="F7">
-        <v>0.2632025810833758</v>
-      </c>
-      <c r="G7">
-        <v>0.16684574059861856</v>
-      </c>
-      <c r="H7">
-        <v>0.78740728797162207</v>
-      </c>
-      <c r="I7">
-        <v>4339</v>
-      </c>
-      <c r="J7">
-        <v>1087</v>
-      </c>
-      <c r="K7">
-        <v>5428</v>
-      </c>
-      <c r="L7">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.73475972151468838</v>
-      </c>
-      <c r="C8">
-        <v>0.8558710667689946</v>
-      </c>
-      <c r="D8">
-        <v>0.82168628940372201</v>
-      </c>
-      <c r="E8">
-        <v>0.78117119641356125</v>
-      </c>
-      <c r="F8">
-        <v>0.26524027848531162</v>
-      </c>
-      <c r="G8">
-        <v>0.14412893323100537</v>
-      </c>
-      <c r="H8">
-        <v>0.7983714930667527</v>
-      </c>
-      <c r="I8">
-        <v>4327</v>
-      </c>
-      <c r="J8">
-        <v>939</v>
-      </c>
-      <c r="K8">
-        <v>5576</v>
-      </c>
-      <c r="L8">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.73713703515028017</v>
-      </c>
-      <c r="C9">
-        <v>0.86492709132770529</v>
-      </c>
-      <c r="D9">
-        <v>0.83144991380961497</v>
-      </c>
-      <c r="E9">
-        <v>0.78449115968258387</v>
-      </c>
-      <c r="F9">
-        <v>0.26286296484971983</v>
-      </c>
-      <c r="G9">
-        <v>0.13507290867229471</v>
-      </c>
-      <c r="H9">
-        <v>0.80425669138987421</v>
-      </c>
-      <c r="I9">
-        <v>4341</v>
-      </c>
-      <c r="J9">
-        <v>880</v>
-      </c>
-      <c r="K9">
-        <v>5635</v>
-      </c>
-      <c r="L9">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.77194769910001693</v>
-      </c>
-      <c r="C10">
-        <v>0.84174980813507294</v>
-      </c>
-      <c r="D10">
-        <v>0.81513358436435357</v>
-      </c>
-      <c r="E10">
-        <v>0.80328108979053758</v>
-      </c>
-      <c r="F10">
-        <v>0.22805230089998302</v>
-      </c>
-      <c r="G10">
-        <v>0.15825019186492709</v>
-      </c>
-      <c r="H10">
-        <v>0.80861012576588198</v>
-      </c>
-      <c r="I10">
-        <v>4546</v>
-      </c>
-      <c r="J10">
-        <v>1031</v>
-      </c>
-      <c r="K10">
-        <v>5484</v>
-      </c>
-      <c r="L10">
-        <v>1343</v>
-      </c>
-    </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.7471557140431313</v>
+        <v>0.77160808286636107</v>
       </c>
       <c r="C11">
-        <v>0.86554105909439749</v>
+        <v>0.84006139677666924</v>
       </c>
       <c r="D11">
-        <v>0.83396512509476872</v>
+        <v>0.81346222699606163</v>
       </c>
       <c r="E11">
-        <v>0.79110549943883279</v>
+        <v>0.80272807274860658</v>
       </c>
       <c r="F11">
-        <v>0.25284428595686875</v>
+        <v>0.22839191713363899</v>
       </c>
       <c r="G11">
-        <v>0.13445894090560245</v>
+        <v>0.15993860322333078</v>
       </c>
       <c r="H11">
-        <v>0.80933569816188322</v>
+        <v>0.8075620767494357</v>
       </c>
       <c r="I11">
-        <v>4400</v>
+        <v>4544</v>
       </c>
       <c r="J11">
-        <v>876</v>
+        <v>1042</v>
       </c>
       <c r="K11">
-        <v>5639</v>
+        <v>5473</v>
       </c>
       <c r="L11">
-        <v>1489</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.74460859229071152</v>
+        <v>0.75038206826286291</v>
       </c>
       <c r="C12">
-        <v>0.86385264773599391</v>
+        <v>0.86047582501918651</v>
       </c>
       <c r="D12">
-        <v>0.83175265553869504</v>
+        <v>0.82939189189189189</v>
       </c>
       <c r="E12">
-        <v>0.78911946158160406</v>
+        <v>0.79225551158846808</v>
       </c>
       <c r="F12">
-        <v>0.25539140770928853</v>
+        <v>0.24961793173713703</v>
       </c>
       <c r="G12">
-        <v>0.13614735226400615</v>
+        <v>0.13952417498081351</v>
       </c>
       <c r="H12">
-        <v>0.80723960012899065</v>
+        <v>0.80820702999032568</v>
       </c>
       <c r="I12">
-        <v>4385</v>
+        <v>4419</v>
       </c>
       <c r="J12">
-        <v>887</v>
+        <v>909</v>
       </c>
       <c r="K12">
-        <v>5628</v>
+        <v>5606</v>
       </c>
       <c r="L12">
-        <v>1504</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.73374087281372047</v>
+        <v>0.73526914586517234</v>
       </c>
       <c r="C13">
-        <v>0.86738296239447432</v>
+        <v>0.86815042210283955</v>
       </c>
       <c r="D13">
-        <v>0.83336547733847632</v>
+        <v>0.83445750626324922</v>
       </c>
       <c r="E13">
-        <v>0.78279540102507272</v>
+        <v>0.78392238392238389</v>
       </c>
       <c r="F13">
-        <v>0.26625912718627953</v>
+        <v>0.26473085413482766</v>
       </c>
       <c r="G13">
-        <v>0.13261703760552571</v>
+        <v>0.1318495778971604</v>
       </c>
       <c r="H13">
-        <v>0.80393421476942917</v>
+        <v>0.80506288294098682</v>
       </c>
       <c r="I13">
-        <v>4321</v>
+        <v>4330</v>
       </c>
       <c r="J13">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="K13">
-        <v>5651</v>
+        <v>5656</v>
       </c>
       <c r="L13">
-        <v>1568</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.75479707930039053</v>
+        <v>0.73832569196807607</v>
       </c>
       <c r="C14">
-        <v>0.84758250191864926</v>
+        <v>0.86231772831926323</v>
       </c>
       <c r="D14">
-        <v>0.81739610150790731</v>
+        <v>0.82897998093422309</v>
       </c>
       <c r="E14">
-        <v>0.79270743611828887</v>
+        <v>0.78474647297108535</v>
       </c>
       <c r="F14">
-        <v>0.24520292069960944</v>
+        <v>0.26167430803192393</v>
       </c>
       <c r="G14">
-        <v>0.15241749808135072</v>
+        <v>0.13768227168073677</v>
       </c>
       <c r="H14">
-        <v>0.80353111899387297</v>
+        <v>0.80345049983876171</v>
       </c>
       <c r="I14">
-        <v>4445</v>
+        <v>4348</v>
       </c>
       <c r="J14">
-        <v>993</v>
+        <v>897</v>
       </c>
       <c r="K14">
-        <v>5522</v>
+        <v>5618</v>
       </c>
       <c r="L14">
-        <v>1444</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.76515537442689763</v>
+        <v>0.73934454066904398</v>
       </c>
       <c r="C15">
-        <v>0.83115886415963158</v>
+        <v>0.85709900230237912</v>
       </c>
       <c r="D15">
-        <v>0.80378166250445948</v>
+        <v>0.82384105960264897</v>
       </c>
       <c r="E15">
-        <v>0.79655781112091795</v>
+        <v>0.78437982862761624</v>
       </c>
       <c r="F15">
-        <v>0.2348446255731024</v>
+        <v>0.26065545933095602</v>
       </c>
       <c r="G15">
-        <v>0.16884113584036839</v>
+        <v>0.14290099769762088</v>
       </c>
       <c r="H15">
-        <v>0.79982263785875529</v>
+        <v>0.80119316349564662</v>
       </c>
       <c r="I15">
-        <v>4506</v>
+        <v>4354</v>
       </c>
       <c r="J15">
-        <v>1100</v>
+        <v>931</v>
       </c>
       <c r="K15">
-        <v>5415</v>
+        <v>5584</v>
       </c>
       <c r="L15">
-        <v>1383</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.73764645950076413</v>
+        <v>0.74019358125318391</v>
       </c>
       <c r="C16">
-        <v>0.85863392171910979</v>
+        <v>0.85326170376055255</v>
       </c>
       <c r="D16">
-        <v>0.8250712250712251</v>
+        <v>0.82013170272812796</v>
       </c>
       <c r="E16">
-        <v>0.78358313489284215</v>
+        <v>0.78417266187050361</v>
       </c>
       <c r="F16">
-        <v>0.26235354049923587</v>
+        <v>0.25980641874681609</v>
       </c>
       <c r="G16">
-        <v>0.14136607828089026</v>
+        <v>0.14673829623944742</v>
       </c>
       <c r="H16">
-        <v>0.80119316349564662</v>
+        <v>0.79958078039342151</v>
       </c>
       <c r="I16">
-        <v>4344</v>
+        <v>4359</v>
       </c>
       <c r="J16">
-        <v>921</v>
+        <v>956</v>
       </c>
       <c r="K16">
-        <v>5594</v>
+        <v>5559</v>
       </c>
       <c r="L16">
-        <v>1545</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.73509933774834435</v>
+        <v>0.77177789098318894</v>
       </c>
       <c r="C17">
-        <v>0.85172678434382199</v>
+        <v>0.81734458940905608</v>
       </c>
       <c r="D17">
-        <v>0.81756373937677052</v>
+        <v>0.79250217959895375</v>
       </c>
       <c r="E17">
-        <v>0.78055985370656911</v>
+        <v>0.79847053531264056</v>
       </c>
       <c r="F17">
-        <v>0.26490066225165565</v>
+        <v>0.228222109016811</v>
       </c>
       <c r="G17">
-        <v>0.14827321565617804</v>
+        <v>0.18265541059094398</v>
       </c>
       <c r="H17">
-        <v>0.79635601418897128</v>
+        <v>0.79571106094808131</v>
       </c>
       <c r="I17">
-        <v>4329</v>
+        <v>4545</v>
       </c>
       <c r="J17">
-        <v>966</v>
+        <v>1190</v>
       </c>
       <c r="K17">
-        <v>5549</v>
+        <v>5325</v>
       </c>
       <c r="L17">
-        <v>1560</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.73645780268296823</v>
+        <v>0.73628799456614025</v>
       </c>
       <c r="C18">
-        <v>0.84927091327705295</v>
+        <v>0.85003837298541829</v>
       </c>
       <c r="D18">
-        <v>0.81537883060725702</v>
+        <v>0.81611142480707699</v>
       </c>
       <c r="E18">
-        <v>0.7809456598447424</v>
+        <v>0.78098998730785507</v>
       </c>
       <c r="F18">
-        <v>0.26354219731703177</v>
+        <v>0.26371200543385975</v>
       </c>
       <c r="G18">
-        <v>0.15072908672294705</v>
+        <v>0.14996162701458174</v>
       </c>
       <c r="H18">
-        <v>0.79571106094808131</v>
+        <v>0.79603353756852624</v>
       </c>
       <c r="I18">
-        <v>4337</v>
+        <v>4336</v>
       </c>
       <c r="J18">
-        <v>982</v>
+        <v>977</v>
       </c>
       <c r="K18">
-        <v>5533</v>
+        <v>5538</v>
       </c>
       <c r="L18">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.74545763287485145</v>
+        <v>0.77313635591781282</v>
       </c>
       <c r="C19">
-        <v>0.84343821949347664</v>
+        <v>0.81059094397544129</v>
       </c>
       <c r="D19">
-        <v>0.81146025878003691</v>
+        <v>0.7867634352859858</v>
       </c>
       <c r="E19">
-        <v>0.78567343437231918</v>
+        <v>0.79809581381290617</v>
       </c>
       <c r="F19">
-        <v>0.25454236712514861</v>
+        <v>0.22686364408218712</v>
       </c>
       <c r="G19">
-        <v>0.15656178050652342</v>
+        <v>0.18940905602455871</v>
       </c>
       <c r="H19">
-        <v>0.79692034827475011</v>
+        <v>0.79280877136407613</v>
       </c>
       <c r="I19">
-        <v>4390</v>
+        <v>4553</v>
       </c>
       <c r="J19">
-        <v>1020</v>
+        <v>1234</v>
       </c>
       <c r="K19">
-        <v>5495</v>
+        <v>5281</v>
       </c>
       <c r="L19">
-        <v>1499</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.739174732552216</v>
+        <v>0.75309899813211068</v>
       </c>
       <c r="C20">
-        <v>0.83975441289332309</v>
+        <v>0.83023791250959322</v>
       </c>
       <c r="D20">
-        <v>0.80655919955530853</v>
+        <v>0.80039704024544311</v>
       </c>
       <c r="E20">
-        <v>0.78079063793349512</v>
+        <v>0.78813929768322888</v>
       </c>
       <c r="F20">
-        <v>0.260825267447784</v>
+        <v>0.2469010018678893</v>
       </c>
       <c r="G20">
-        <v>0.16024558710667691</v>
+        <v>0.16976208749040675</v>
       </c>
       <c r="H20">
-        <v>0.79200257981296351</v>
+        <v>0.79361496291518863</v>
       </c>
       <c r="I20">
-        <v>4353</v>
+        <v>4435</v>
       </c>
       <c r="J20">
-        <v>1044</v>
+        <v>1106</v>
       </c>
       <c r="K20">
-        <v>5471</v>
+        <v>5409</v>
       </c>
       <c r="L20">
-        <v>1536</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.72270334521990154</v>
+        <v>0.71879775853285788</v>
       </c>
       <c r="C21">
-        <v>0.85786646201074446</v>
+        <v>0.86170376055257103</v>
       </c>
       <c r="D21">
-        <v>0.82130451563103046</v>
+        <v>0.82450331125827814</v>
       </c>
       <c r="E21">
-        <v>0.77388535031847139</v>
+        <v>0.77221458046767533</v>
       </c>
       <c r="F21">
-        <v>0.27729665478009846</v>
+        <v>0.28120224146714212</v>
       </c>
       <c r="G21">
-        <v>0.14213353798925557</v>
+        <v>0.138296239447429</v>
       </c>
       <c r="H21">
-        <v>0.79369558207029989</v>
+        <v>0.79385682038052241</v>
       </c>
       <c r="I21">
-        <v>4256</v>
+        <v>4233</v>
       </c>
       <c r="J21">
-        <v>926</v>
+        <v>901</v>
       </c>
       <c r="K21">
-        <v>5589</v>
+        <v>5614</v>
       </c>
       <c r="L21">
-        <v>1633</v>
+        <v>1656</v>
       </c>
     </row>
   </sheetData>
@@ -1016,7 +1031,7 @@
   <cols>
     <col min="1" max="1" width="13" customWidth="true"/>
     <col min="2" max="2" width="12.7109375" customWidth="true"/>
-    <col min="3" max="3" width="13.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
@@ -1029,45 +1044,45 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1102,457 +1117,463 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.49596774193548387</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C3">
-        <v>0.89210155148095904</v>
+        <v>0.92877291960507757</v>
       </c>
       <c r="D3">
-        <v>0.80078125</v>
+        <v>0.81121495327102799</v>
       </c>
       <c r="E3">
-        <v>0.6693121693121693</v>
+        <v>0.62034856335374466</v>
       </c>
       <c r="F3">
-        <v>0.50403225806451613</v>
+        <v>0.65000000000000002</v>
       </c>
       <c r="G3">
-        <v>0.1078984485190409</v>
+        <v>0.071227080394922426</v>
       </c>
       <c r="H3">
-        <v>0.70729872084273893</v>
+        <v>0.6587659894657637</v>
       </c>
       <c r="I3">
-        <v>615</v>
+        <v>434</v>
       </c>
       <c r="J3">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="K3">
-        <v>1265</v>
+        <v>1317</v>
       </c>
       <c r="L3">
-        <v>625</v>
+        <v>806</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7129032258064516</v>
+        <v>0.70241935483870965</v>
       </c>
       <c r="C4">
-        <v>0.77009873060648804</v>
+        <v>0.78138222849083216</v>
       </c>
       <c r="D4">
-        <v>0.73057851239669425</v>
+        <v>0.73751058425063509</v>
       </c>
       <c r="E4">
-        <v>0.7541436464088398</v>
+        <v>0.75016926201760326</v>
       </c>
       <c r="F4">
-        <v>0.2870967741935484</v>
+        <v>0.29758064516129035</v>
       </c>
       <c r="G4">
-        <v>0.22990126939351199</v>
+        <v>0.21861777150916784</v>
       </c>
       <c r="H4">
-        <v>0.74341610233258093</v>
+        <v>0.74454477050413848</v>
       </c>
       <c r="I4">
-        <v>884</v>
+        <v>871</v>
       </c>
       <c r="J4">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="K4">
-        <v>1092</v>
+        <v>1108</v>
       </c>
       <c r="L4">
-        <v>356</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.73790322580645162</v>
+        <v>0.73467741935483866</v>
       </c>
       <c r="C5">
-        <v>0.76939351198871653</v>
+        <v>0.77150916784203105</v>
       </c>
       <c r="D5">
-        <v>0.73671497584541068</v>
+        <v>0.73765182186234812</v>
       </c>
       <c r="E5">
-        <v>0.77048022598870058</v>
+        <v>0.76879831342234717</v>
       </c>
       <c r="F5">
-        <v>0.26209677419354838</v>
+        <v>0.26532258064516129</v>
       </c>
       <c r="G5">
-        <v>0.2306064880112835</v>
+        <v>0.22849083215796898</v>
       </c>
       <c r="H5">
-        <v>0.75470278404815649</v>
+        <v>0.75432656132430398</v>
       </c>
       <c r="I5">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="J5">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K5">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="L5">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.7290322580645161</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="C6">
-        <v>0.81382228490832154</v>
+        <v>0.81593794076163606</v>
       </c>
       <c r="D6">
-        <v>0.77397260273972601</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="E6">
-        <v>0.77449664429530196</v>
+        <v>0.77236315086782381</v>
       </c>
       <c r="F6">
-        <v>0.2709677419354839</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G6">
-        <v>0.18617771509167841</v>
+        <v>0.18406205923836388</v>
       </c>
       <c r="H6">
-        <v>0.77426636568848761</v>
+        <v>0.77351392024078258</v>
       </c>
       <c r="I6">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="J6">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="K6">
-        <v>1154</v>
+        <v>1157</v>
       </c>
       <c r="L6">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.72258064516129028</v>
+        <v>0.72016129032258069</v>
       </c>
       <c r="C7">
-        <v>0.83850493653032443</v>
+        <v>0.844851904090268</v>
       </c>
       <c r="D7">
-        <v>0.7964444444444444</v>
+        <v>0.80233602875112309</v>
       </c>
       <c r="E7">
-        <v>0.77560339204174822</v>
+        <v>0.77540453074433657</v>
       </c>
       <c r="F7">
-        <v>0.27741935483870966</v>
+        <v>0.27983870967741936</v>
       </c>
       <c r="G7">
-        <v>0.1614950634696756</v>
+        <v>0.15514809590973203</v>
       </c>
       <c r="H7">
-        <v>0.78442437923250563</v>
+        <v>0.78668171557562072</v>
       </c>
       <c r="I7">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="J7">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="K7">
-        <v>1189</v>
+        <v>1198</v>
       </c>
       <c r="L7">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.72177419354838712</v>
+        <v>0.72016129032258069</v>
       </c>
       <c r="C8">
-        <v>0.85895627644569816</v>
+        <v>0.85684062059238364</v>
       </c>
       <c r="D8">
-        <v>0.81735159817351599</v>
+        <v>0.81478102189781021</v>
       </c>
       <c r="E8">
-        <v>0.77927063339731284</v>
+        <v>0.77784891165172854</v>
       </c>
       <c r="F8">
-        <v>0.27822580645161288</v>
+        <v>0.27983870967741936</v>
       </c>
       <c r="G8">
-        <v>0.14104372355430184</v>
+        <v>0.14315937940761636</v>
       </c>
       <c r="H8">
-        <v>0.79495861550037628</v>
+        <v>0.79307750188111359</v>
       </c>
       <c r="I8">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="J8">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="K8">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="L8">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.72983870967741937</v>
+        <v>0.7314516129032258</v>
       </c>
       <c r="C9">
-        <v>0.86600846262341324</v>
+        <v>0.86812411847672777</v>
       </c>
       <c r="D9">
-        <v>0.82648401826484019</v>
+        <v>0.82906764168190128</v>
       </c>
       <c r="E9">
-        <v>0.78566858605246326</v>
+        <v>0.78708439897698212</v>
       </c>
       <c r="F9">
-        <v>0.27016129032258063</v>
+        <v>0.2685483870967742</v>
       </c>
       <c r="G9">
-        <v>0.13399153737658676</v>
+        <v>0.1318758815232722</v>
       </c>
       <c r="H9">
-        <v>0.80248306997742669</v>
+        <v>0.80436418359668926</v>
       </c>
       <c r="I9">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="J9">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K9">
-        <v>1228</v>
+        <v>1231</v>
       </c>
       <c r="L9">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.76532258064516134</v>
+        <v>0.73548387096774193</v>
       </c>
       <c r="C10">
-        <v>0.84908321579689705</v>
+        <v>0.87376586741889983</v>
       </c>
       <c r="D10">
-        <v>0.81599312123817713</v>
+        <v>0.83593033913840509</v>
       </c>
       <c r="E10">
-        <v>0.80535117056856187</v>
+        <v>0.7906828334396937</v>
       </c>
       <c r="F10">
-        <v>0.23467741935483871</v>
+        <v>0.26451612903225807</v>
       </c>
       <c r="G10">
-        <v>0.15091678420310295</v>
+        <v>0.12623413258110014</v>
       </c>
       <c r="H10">
-        <v>0.8100075244544771</v>
+        <v>0.80925507900677196</v>
       </c>
       <c r="I10">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="J10">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="K10">
-        <v>1204</v>
+        <v>1239</v>
       </c>
       <c r="L10">
-        <v>291</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.64919354838709675</v>
+        <v>0.65080645161290318</v>
       </c>
       <c r="C11">
-        <v>0.91607898448519043</v>
+        <v>0.91466854724964741</v>
       </c>
       <c r="D11">
-        <v>0.87121212121212122</v>
+        <v>0.86961206896551724</v>
       </c>
       <c r="E11">
-        <v>0.74913494809688586</v>
+        <v>0.74971098265895952</v>
       </c>
       <c r="F11">
-        <v>0.35080645161290325</v>
+        <v>0.34919354838709676</v>
       </c>
       <c r="G11">
-        <v>0.083921015514809585</v>
+        <v>0.085331452750352615</v>
       </c>
       <c r="H11">
         <v>0.79157261098570353</v>
       </c>
       <c r="I11">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="J11">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K11">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="L11">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.29677419354838708</v>
       </c>
       <c r="C12">
-        <v>0.012693935119887164</v>
+        <v>0.98519040902679833</v>
       </c>
       <c r="D12">
-        <v>0.46969696969696972</v>
+        <v>0.94601542416452444</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.61568973115910097</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.70322580645161292</v>
       </c>
       <c r="G12">
-        <v>0.98730606488011285</v>
+        <v>0.014809590973201692</v>
       </c>
       <c r="H12">
-        <v>0.47328818660647104</v>
+        <v>0.66403310759969902</v>
       </c>
       <c r="I12">
-        <v>1240</v>
+        <v>368</v>
       </c>
       <c r="J12">
-        <v>1400</v>
+        <v>21</v>
       </c>
       <c r="K12">
-        <v>18</v>
+        <v>1397</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>872</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.66774193548387095</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.89703808180535971</v>
       </c>
       <c r="D13">
-        <v>0.46651617757712566</v>
+        <v>0.85010266940451751</v>
+      </c>
+      <c r="E13">
+        <v>0.75534441805225649</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.33225806451612905</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.10296191819464035</v>
       </c>
       <c r="H13">
-        <v>0.46651617757712566</v>
+        <v>0.79006772009029347</v>
       </c>
       <c r="I13">
-        <v>1240</v>
+        <v>828</v>
       </c>
       <c r="J13">
-        <v>1418</v>
+        <v>146</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1272</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.85241935483870968</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.47602256699576867</v>
       </c>
       <c r="D14">
-        <v>0.46651617757712566</v>
+        <v>0.5872222222222222</v>
+      </c>
+      <c r="E14">
+        <v>0.78671328671328666</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.14758064516129032</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.52397743300423127</v>
       </c>
       <c r="H14">
-        <v>0.46651617757712566</v>
+        <v>0.6516177577125658</v>
       </c>
       <c r="I14">
-        <v>1240</v>
+        <v>1057</v>
       </c>
       <c r="J14">
-        <v>1418</v>
+        <v>743</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1587,7 +1608,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -1622,7 +1643,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -1657,7 +1678,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1692,7 +1713,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -1727,42 +1748,42 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0.46651617757712566</v>
+      <c r="E20">
+        <v>0.53348382242287429</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0.46651617757712566</v>
+        <v>0.53348382242287429</v>
       </c>
       <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1418</v>
+      </c>
+      <c r="L20">
         <v>1240</v>
       </c>
-      <c r="J20">
-        <v>1418</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -1811,342 +1832,345 @@
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true"/>
     <col min="8" max="8" width="12.7109375" customWidth="true"/>
     <col min="9" max="9" width="4.140625" customWidth="true"/>
     <col min="10" max="10" width="4.140625" customWidth="true"/>
     <col min="11" max="11" width="5.140625" customWidth="true"/>
-    <col min="12" max="12" width="5.140625" customWidth="true"/>
+    <col min="12" max="12" width="4.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.57653457653457651</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.65499635302698755</v>
+      </c>
+      <c r="D2">
+        <v>0.61069958847736627</v>
       </c>
       <c r="E2">
-        <v>0.51580135440180586</v>
+        <v>0.62231462231462231</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.42346542346542349</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.34500364697301239</v>
       </c>
       <c r="H2">
-        <v>0.51580135440180586</v>
+        <v>0.61700526711813397</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>742</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="K2">
-        <v>1371</v>
+        <v>898</v>
       </c>
       <c r="L2">
-        <v>1287</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.51126651126651124</v>
+        <v>0.3504273504273504</v>
       </c>
       <c r="C3">
-        <v>0.87892049598832966</v>
+        <v>0.91976659372720637</v>
       </c>
       <c r="D3">
-        <v>0.79854368932038833</v>
+        <v>0.80392156862745101</v>
       </c>
       <c r="E3">
-        <v>0.6570338058887677</v>
+        <v>0.60133524082021939</v>
       </c>
       <c r="F3">
-        <v>0.48873348873348871</v>
+        <v>0.6495726495726496</v>
       </c>
       <c r="G3">
-        <v>0.12107950401167031</v>
+        <v>0.080233406272793587</v>
       </c>
       <c r="H3">
-        <v>0.70090293453724606</v>
+        <v>0.64409330323551539</v>
       </c>
       <c r="I3">
-        <v>658</v>
+        <v>451</v>
       </c>
       <c r="J3">
-        <v>166</v>
+        <v>110</v>
       </c>
       <c r="K3">
-        <v>1205</v>
+        <v>1261</v>
       </c>
       <c r="L3">
-        <v>629</v>
+        <v>836</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.6806526806526807</v>
+        <v>0.68220668220668224</v>
       </c>
       <c r="C4">
-        <v>0.80743982494529543</v>
+        <v>0.80598103574033553</v>
       </c>
       <c r="D4">
-        <v>0.76842105263157889</v>
+        <v>0.7674825174825175</v>
       </c>
       <c r="E4">
-        <v>0.72924901185770752</v>
+        <v>0.72985468956406874</v>
       </c>
       <c r="F4">
-        <v>0.31934731934731936</v>
+        <v>0.31779331779331782</v>
       </c>
       <c r="G4">
-        <v>0.1925601750547046</v>
+        <v>0.19401896425966447</v>
       </c>
       <c r="H4">
         <v>0.74604966139954854</v>
       </c>
       <c r="I4">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="J4">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="K4">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="L4">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.75291375291375295</v>
+        <v>0.75058275058275059</v>
       </c>
       <c r="C5">
-        <v>0.76513493800145882</v>
+        <v>0.76805251641137851</v>
       </c>
       <c r="D5">
-        <v>0.75058094500387296</v>
+        <v>0.75233644859813087</v>
       </c>
       <c r="E5">
-        <v>0.76737381126554494</v>
+        <v>0.76637554585152834</v>
       </c>
       <c r="F5">
-        <v>0.24708624708624707</v>
+        <v>0.24941724941724941</v>
       </c>
       <c r="G5">
-        <v>0.23486506199854121</v>
+        <v>0.23194748358862144</v>
       </c>
       <c r="H5">
-        <v>0.75921745673438679</v>
+        <v>0.7595936794582393</v>
       </c>
       <c r="I5">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="J5">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="K5">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="L5">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.73892773892773889</v>
       </c>
       <c r="C6">
-        <v>0.80962800875273522</v>
+        <v>0.81327498176513491</v>
       </c>
       <c r="D6">
-        <v>0.78465346534653468</v>
+        <v>0.78790389395194693</v>
       </c>
       <c r="E6">
-        <v>0.76763485477178428</v>
+        <v>0.76843556168159888</v>
       </c>
       <c r="F6">
         <v>0.26107226107226106</v>
       </c>
       <c r="G6">
-        <v>0.19037199124726478</v>
+        <v>0.18672501823486506</v>
       </c>
       <c r="H6">
-        <v>0.77539503386004516</v>
+        <v>0.77727614747930773</v>
       </c>
       <c r="I6">
         <v>951</v>
       </c>
       <c r="J6">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="K6">
-        <v>1110</v>
+        <v>1115</v>
       </c>
       <c r="L6">
         <v>336</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.7350427350427351</v>
+        <v>0.73193473193473191</v>
       </c>
       <c r="C7">
-        <v>0.82567469000729399</v>
+        <v>0.83005105762217357</v>
       </c>
       <c r="D7">
-        <v>0.79831223628691983</v>
+        <v>0.80170212765957449</v>
       </c>
       <c r="E7">
-        <v>0.76849966055668706</v>
+        <v>0.76736345246122728</v>
       </c>
       <c r="F7">
-        <v>0.26495726495726496</v>
+        <v>0.26806526806526809</v>
       </c>
       <c r="G7">
-        <v>0.17432530999270604</v>
+        <v>0.1699489423778264</v>
       </c>
       <c r="H7">
-        <v>0.78179082016553803</v>
+        <v>0.78254326561324306</v>
       </c>
       <c r="I7">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="J7">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K7">
-        <v>1132</v>
+        <v>1138</v>
       </c>
       <c r="L7">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.73581973581973581</v>
+        <v>0.73348873348873345</v>
       </c>
       <c r="C8">
-        <v>0.84463894967177244</v>
+        <v>0.83880379285193285</v>
       </c>
       <c r="D8">
-        <v>0.81637931034482758</v>
+        <v>0.81030042918454936</v>
       </c>
       <c r="E8">
-        <v>0.77303070761014692</v>
+        <v>0.77026121902210309</v>
       </c>
       <c r="F8">
-        <v>0.26418026418026419</v>
+        <v>0.2665112665112665</v>
       </c>
       <c r="G8">
-        <v>0.15536105032822758</v>
+        <v>0.16119620714806709</v>
       </c>
       <c r="H8">
-        <v>0.79194883370955604</v>
+        <v>0.78781038374717838</v>
       </c>
       <c r="I8">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="J8">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="K8">
-        <v>1158</v>
+        <v>1150</v>
       </c>
       <c r="L8">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.73348873348873345</v>
+        <v>0.73426573426573427</v>
       </c>
       <c r="C9">
         <v>0.85412107950401162</v>
       </c>
       <c r="D9">
-        <v>0.82517482517482521</v>
+        <v>0.8253275109170306</v>
       </c>
       <c r="E9">
-        <v>0.77344782034346105</v>
+        <v>0.77395902181097154</v>
       </c>
       <c r="F9">
-        <v>0.2665112665112665</v>
+        <v>0.26573426573426573</v>
       </c>
       <c r="G9">
         <v>0.14587892049598833</v>
       </c>
       <c r="H9">
-        <v>0.79571106094808131</v>
+        <v>0.79608728367193382</v>
       </c>
       <c r="I9">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="J9">
         <v>200</v>
@@ -2155,150 +2179,150 @@
         <v>1171</v>
       </c>
       <c r="L9">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>0.73581973581973581</v>
+      </c>
+      <c r="C10">
+        <v>0.86141502552881111</v>
+      </c>
+      <c r="D10">
+        <v>0.83289357959542654</v>
+      </c>
+      <c r="E10">
+        <v>0.77646285338593035</v>
+      </c>
+      <c r="F10">
+        <v>0.26418026418026419</v>
+      </c>
+      <c r="G10">
+        <v>0.13858497447118892</v>
+      </c>
+      <c r="H10">
+        <v>0.800601956358164</v>
+      </c>
+      <c r="I10">
+        <v>947</v>
+      </c>
+      <c r="J10">
+        <v>190</v>
+      </c>
+      <c r="K10">
+        <v>1181</v>
+      </c>
+      <c r="L10">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>0.77466977466977471</v>
       </c>
-      <c r="C10">
-        <v>0.83296863603209337</v>
-      </c>
-      <c r="D10">
-        <v>0.81321370309951058</v>
-      </c>
-      <c r="E10">
-        <v>0.79748603351955305</v>
-      </c>
-      <c r="F10">
+      <c r="C11">
+        <v>0.83005105762217357</v>
+      </c>
+      <c r="D11">
+        <v>0.81056910569105689</v>
+      </c>
+      <c r="E11">
+        <v>0.79691876750700286</v>
+      </c>
+      <c r="F11">
         <v>0.22533022533022534</v>
       </c>
-      <c r="G10">
-        <v>0.16703136396790663</v>
-      </c>
-      <c r="H10">
-        <v>0.80474040632054178</v>
-      </c>
-      <c r="I10">
+      <c r="G11">
+        <v>0.1699489423778264</v>
+      </c>
+      <c r="H11">
+        <v>0.80323551542513172</v>
+      </c>
+      <c r="I11">
         <v>997</v>
       </c>
-      <c r="J10">
-        <v>229</v>
-      </c>
-      <c r="K10">
-        <v>1142</v>
-      </c>
-      <c r="L10">
+      <c r="J11">
+        <v>233</v>
+      </c>
+      <c r="K11">
+        <v>1138</v>
+      </c>
+      <c r="L11">
         <v>290</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0.74203574203574207</v>
-      </c>
-      <c r="C11">
-        <v>0.85849744711889131</v>
-      </c>
-      <c r="D11">
-        <v>0.83115752828546563</v>
-      </c>
-      <c r="E11">
-        <v>0.77998674618952946</v>
-      </c>
-      <c r="F11">
-        <v>0.25796425796425798</v>
-      </c>
-      <c r="G11">
-        <v>0.14150255288110869</v>
-      </c>
-      <c r="H11">
-        <v>0.80210684725357406</v>
-      </c>
-      <c r="I11">
-        <v>955</v>
-      </c>
-      <c r="J11">
-        <v>194</v>
-      </c>
-      <c r="K11">
-        <v>1177</v>
-      </c>
-      <c r="L11">
-        <v>332</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.74125874125874125</v>
+        <v>0.74825174825174823</v>
       </c>
       <c r="C12">
-        <v>0.85557986870897151</v>
+        <v>0.84609773887673234</v>
       </c>
       <c r="D12">
-        <v>0.828125</v>
+        <v>0.82027257240204432</v>
       </c>
       <c r="E12">
-        <v>0.7788844621513944</v>
+        <v>0.78167115902964956</v>
       </c>
       <c r="F12">
-        <v>0.25874125874125875</v>
+        <v>0.25174825174825177</v>
       </c>
       <c r="G12">
-        <v>0.14442013129102846</v>
+        <v>0.15390226112326769</v>
       </c>
       <c r="H12">
-        <v>0.80022573363431149</v>
+        <v>0.79872084273890143</v>
       </c>
       <c r="I12">
-        <v>954</v>
+        <v>963</v>
       </c>
       <c r="J12">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="K12">
-        <v>1173</v>
+        <v>1160</v>
       </c>
       <c r="L12">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.73193473193473191</v>
+        <v>0.73271173271173273</v>
       </c>
       <c r="C13">
         <v>0.85630926331145152</v>
       </c>
       <c r="D13">
-        <v>0.82704126426690083</v>
+        <v>0.82719298245614037</v>
       </c>
       <c r="E13">
-        <v>0.77287689269256088</v>
+        <v>0.77338603425559949</v>
       </c>
       <c r="F13">
-        <v>0.26806526806526809</v>
+        <v>0.26728826728826727</v>
       </c>
       <c r="G13">
         <v>0.14369073668854851</v>
       </c>
       <c r="H13">
-        <v>0.79608728367193382</v>
+        <v>0.79646350639578634</v>
       </c>
       <c r="I13">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="J13">
         <v>197</v>
@@ -2307,311 +2331,311 @@
         <v>1174</v>
       </c>
       <c r="L13">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.75446775446775449</v>
+        <v>0.73659673659673663</v>
       </c>
       <c r="C14">
-        <v>0.83661560904449306</v>
+        <v>0.85193289569657182</v>
       </c>
       <c r="D14">
-        <v>0.81255230125523015</v>
+        <v>0.82363162467419637</v>
       </c>
       <c r="E14">
-        <v>0.78400546821599448</v>
+        <v>0.77504976775049772</v>
       </c>
       <c r="F14">
-        <v>0.24553224553224554</v>
+        <v>0.26340326340326342</v>
       </c>
       <c r="G14">
-        <v>0.16338439095550694</v>
+        <v>0.14806710430342815</v>
       </c>
       <c r="H14">
-        <v>0.79683972911963885</v>
+        <v>0.79608728367193382</v>
       </c>
       <c r="I14">
-        <v>971</v>
+        <v>948</v>
       </c>
       <c r="J14">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="K14">
-        <v>1147</v>
+        <v>1168</v>
       </c>
       <c r="L14">
-        <v>316</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.76379176379176383</v>
+        <v>0.73815073815073817</v>
       </c>
       <c r="C15">
-        <v>0.82567469000729399</v>
+        <v>0.84536834427425234</v>
       </c>
       <c r="D15">
-        <v>0.80441898527004907</v>
+        <v>0.81755593803786575</v>
       </c>
       <c r="E15">
-        <v>0.78830083565459608</v>
+        <v>0.77473262032085566</v>
       </c>
       <c r="F15">
-        <v>0.23620823620823622</v>
+        <v>0.26184926184926183</v>
       </c>
       <c r="G15">
-        <v>0.17432530999270604</v>
+        <v>0.15463165572574764</v>
       </c>
       <c r="H15">
-        <v>0.79571106094808131</v>
+        <v>0.7934537246049661</v>
       </c>
       <c r="I15">
-        <v>983</v>
+        <v>950</v>
       </c>
       <c r="J15">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="K15">
-        <v>1132</v>
+        <v>1159</v>
       </c>
       <c r="L15">
-        <v>304</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.73737373737373735</v>
+        <v>0.74203574203574207</v>
       </c>
       <c r="C16">
-        <v>0.84536834427425234</v>
+        <v>0.84245076586433265</v>
       </c>
       <c r="D16">
-        <v>0.81739879414298022</v>
+        <v>0.81554227156276682</v>
       </c>
       <c r="E16">
-        <v>0.77421509686038747</v>
+        <v>0.77673167451244118</v>
       </c>
       <c r="F16">
-        <v>0.26262626262626265</v>
+        <v>0.25796425796425798</v>
       </c>
       <c r="G16">
-        <v>0.15463165572574764</v>
+        <v>0.1575492341356674</v>
       </c>
       <c r="H16">
-        <v>0.79307750188111359</v>
+        <v>0.79382994732881862</v>
       </c>
       <c r="I16">
-        <v>949</v>
+        <v>955</v>
       </c>
       <c r="J16">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K16">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="L16">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B17">
+        <v>0.77311577311577306</v>
+      </c>
+      <c r="C17">
+        <v>0.80306345733041573</v>
+      </c>
+      <c r="D17">
+        <v>0.7865612648221344</v>
+      </c>
+      <c r="E17">
+        <v>0.79038047379755927</v>
+      </c>
+      <c r="F17">
+        <v>0.22688422688422688</v>
+      </c>
+      <c r="G17">
+        <v>0.19693654266958424</v>
+      </c>
+      <c r="H17">
+        <v>0.78856282919488341</v>
+      </c>
+      <c r="I17">
+        <v>995</v>
+      </c>
+      <c r="J17">
+        <v>270</v>
+      </c>
+      <c r="K17">
+        <v>1101</v>
+      </c>
+      <c r="L17">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>0.73581973581973581</v>
       </c>
-      <c r="C17">
-        <v>0.84099197665937275</v>
-      </c>
-      <c r="D17">
-        <v>0.81287553648068667</v>
-      </c>
-      <c r="E17">
-        <v>0.77227059611520432</v>
-      </c>
-      <c r="F17">
+      <c r="C18">
+        <v>0.83734500364697306</v>
+      </c>
+      <c r="D18">
+        <v>0.80940170940170941</v>
+      </c>
+      <c r="E18">
+        <v>0.771505376344086</v>
+      </c>
+      <c r="F18">
         <v>0.26418026418026419</v>
       </c>
-      <c r="G17">
-        <v>0.15900802334062727</v>
-      </c>
-      <c r="H17">
-        <v>0.79006772009029347</v>
-      </c>
-      <c r="I17">
+      <c r="G18">
+        <v>0.16265499635302699</v>
+      </c>
+      <c r="H18">
+        <v>0.78818660647103089</v>
+      </c>
+      <c r="I18">
         <v>947</v>
       </c>
-      <c r="J17">
-        <v>218</v>
-      </c>
-      <c r="K17">
-        <v>1153</v>
-      </c>
-      <c r="L17">
+      <c r="J18">
+        <v>223</v>
+      </c>
+      <c r="K18">
+        <v>1148</v>
+      </c>
+      <c r="L18">
         <v>340</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0.73737373737373735</v>
-      </c>
-      <c r="C18">
-        <v>0.83661560904449306</v>
-      </c>
-      <c r="D18">
-        <v>0.80903665814151748</v>
-      </c>
-      <c r="E18">
-        <v>0.77239057239057241</v>
-      </c>
-      <c r="F18">
-        <v>0.26262626262626265</v>
-      </c>
-      <c r="G18">
-        <v>0.16338439095550694</v>
-      </c>
-      <c r="H18">
-        <v>0.78856282919488341</v>
-      </c>
-      <c r="I18">
-        <v>949</v>
-      </c>
-      <c r="J18">
-        <v>224</v>
-      </c>
-      <c r="K18">
-        <v>1147</v>
-      </c>
-      <c r="L18">
-        <v>338</v>
-      </c>
-    </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.74592074592074598</v>
+        <v>0.77466977466977471</v>
       </c>
       <c r="C19">
-        <v>0.83223924142961347</v>
+        <v>0.79795769511305614</v>
       </c>
       <c r="D19">
-        <v>0.80672268907563027</v>
+        <v>0.78257456828885397</v>
       </c>
       <c r="E19">
-        <v>0.77724795640326971</v>
+        <v>0.79046242774566478</v>
       </c>
       <c r="F19">
-        <v>0.25407925407925408</v>
+        <v>0.22533022533022534</v>
       </c>
       <c r="G19">
-        <v>0.16776075857038658</v>
+        <v>0.20204230488694383</v>
       </c>
       <c r="H19">
-        <v>0.79044394281414598</v>
+        <v>0.78668171557562072</v>
       </c>
       <c r="I19">
-        <v>960</v>
+        <v>997</v>
       </c>
       <c r="J19">
-        <v>230</v>
+        <v>277</v>
       </c>
       <c r="K19">
-        <v>1141</v>
+        <v>1094</v>
       </c>
       <c r="L19">
-        <v>327</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.73815073815073817</v>
+        <v>0.74980574980574977</v>
       </c>
       <c r="C20">
-        <v>0.82713347921225377</v>
+        <v>0.8169219547775346</v>
       </c>
       <c r="D20">
-        <v>0.80033698399326036</v>
+        <v>0.79358552631578949</v>
       </c>
       <c r="E20">
-        <v>0.77090414683888508</v>
+        <v>0.77669902912621358</v>
       </c>
       <c r="F20">
-        <v>0.26184926184926183</v>
+        <v>0.25019425019425018</v>
       </c>
       <c r="G20">
-        <v>0.17286652078774617</v>
+        <v>0.18307804522246535</v>
       </c>
       <c r="H20">
-        <v>0.78404815650865312</v>
+        <v>0.78442437923250563</v>
       </c>
       <c r="I20">
-        <v>950</v>
+        <v>965</v>
       </c>
       <c r="J20">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="K20">
-        <v>1134</v>
+        <v>1120</v>
       </c>
       <c r="L20">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.72183372183372185</v>
+        <v>0.71717171717171713</v>
       </c>
       <c r="C21">
-        <v>0.84463894967177244</v>
+        <v>0.84609773887673234</v>
       </c>
       <c r="D21">
-        <v>0.81348511383537658</v>
+        <v>0.81393298059964725</v>
       </c>
       <c r="E21">
-        <v>0.76385224274406327</v>
+        <v>0.76115485564304464</v>
       </c>
       <c r="F21">
-        <v>0.27816627816627815</v>
+        <v>0.28282828282828282</v>
       </c>
       <c r="G21">
-        <v>0.15536105032822758</v>
+        <v>0.15390226112326769</v>
       </c>
       <c r="H21">
-        <v>0.78517682468021066</v>
+        <v>0.7836719337848006</v>
       </c>
       <c r="I21">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="J21">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K21">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="L21">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>